<commit_message>
Created a new combined Excel file for football club stats
</commit_message>
<xml_diff>
--- a/Football Club Stats.zip_unzipped/Football Club Stats/Luton Stats.xlsx
+++ b/Football Club Stats.zip_unzipped/Football Club Stats/Luton Stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -579,206 +579,6 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>23/24</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Luton</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>18</v>
-      </c>
-      <c r="D4" t="n">
-        <v>26</v>
-      </c>
-      <c r="E4" t="n">
-        <v>38</v>
-      </c>
-      <c r="F4" t="n">
-        <v>6</v>
-      </c>
-      <c r="G4" t="n">
-        <v>24</v>
-      </c>
-      <c r="H4" t="n">
-        <v>8</v>
-      </c>
-      <c r="I4" t="n">
-        <v>52</v>
-      </c>
-      <c r="J4" t="n">
-        <v>85</v>
-      </c>
-      <c r="K4" t="n">
-        <v>-33</v>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Carlton Morris</t>
-        </is>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>23/24</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Luton</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>18</v>
-      </c>
-      <c r="D5" t="n">
-        <v>26</v>
-      </c>
-      <c r="E5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F5" t="n">
-        <v>6</v>
-      </c>
-      <c r="G5" t="n">
-        <v>24</v>
-      </c>
-      <c r="H5" t="n">
-        <v>8</v>
-      </c>
-      <c r="I5" t="n">
-        <v>52</v>
-      </c>
-      <c r="J5" t="n">
-        <v>85</v>
-      </c>
-      <c r="K5" t="n">
-        <v>-33</v>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Carlton Morris</t>
-        </is>
-      </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" t="n">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>23/24</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Luton</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>18</v>
-      </c>
-      <c r="D6" t="n">
-        <v>26</v>
-      </c>
-      <c r="E6" t="n">
-        <v>38</v>
-      </c>
-      <c r="F6" t="n">
-        <v>6</v>
-      </c>
-      <c r="G6" t="n">
-        <v>24</v>
-      </c>
-      <c r="H6" t="n">
-        <v>8</v>
-      </c>
-      <c r="I6" t="n">
-        <v>52</v>
-      </c>
-      <c r="J6" t="n">
-        <v>85</v>
-      </c>
-      <c r="K6" t="n">
-        <v>-33</v>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>Carlton Morris</t>
-        </is>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>23/24</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Luton</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>18</v>
-      </c>
-      <c r="D7" t="n">
-        <v>26</v>
-      </c>
-      <c r="E7" t="n">
-        <v>38</v>
-      </c>
-      <c r="F7" t="n">
-        <v>6</v>
-      </c>
-      <c r="G7" t="n">
-        <v>24</v>
-      </c>
-      <c r="H7" t="n">
-        <v>8</v>
-      </c>
-      <c r="I7" t="n">
-        <v>52</v>
-      </c>
-      <c r="J7" t="n">
-        <v>85</v>
-      </c>
-      <c r="K7" t="n">
-        <v>-33</v>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>Carlton Morris</t>
-        </is>
-      </c>
-      <c r="M7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" t="n">
-        <v>71</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>